<commit_message>
Add support for #ignore part way through lines in the framework
</commit_message>
<xml_diff>
--- a/tests/sir_framework_ignore.xlsx
+++ b/tests/sir_framework_ignore.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romesh\projects\atomica\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3EDDDCF-35A0-4E49-AF7F-7DF67EA369B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1AAF564-B58C-47E5-AD40-9BD29F9F2D34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3255" yWindow="1470" windowWidth="32385" windowHeight="15690" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3255" yWindow="1470" windowWidth="32385" windowHeight="15690" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -354,7 +354,49 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000004000000}">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000005000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>This column, and any that immediately follow without a specified
+header, is for the 'components' of a cascade characteristic.
+A component is either a compartment or a characteristic that has
+been previously defined, i.e. in a previous row, and should be
+listed in this (and appropriate subsequent columns) by 'Code Name'.
+For example, characteristic 'infected' may include 'dis_stage_1',
+'dis_stage_2' and 'dis_advanced', where 'dis_advanced' is another
+previously-defined characteristic including 'dis_stage_3' and
+'dis_stage_4'.
+In an example model, 'infected' would track population size summed
+across the four 'dis_stage' states.
+Note: If two or more components are listed in the same column, they
+must be separated by a comma.
+Whitespace is allowable and will be deleted during processing.
+[attribute_charac_includes]</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000006000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>This column defines a 'denominator' attribute for a 'charac' item.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000004000000}">
       <text>
         <r>
           <rPr>
@@ -382,48 +424,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000005000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>This column, and any that immediately follow without a specified
-header, is for the 'components' of a cascade characteristic.
-A component is either a compartment or a characteristic that has
-been previously defined, i.e. in a previous row, and should be
-listed in this (and appropriate subsequent columns) by 'Code Name'.
-For example, characteristic 'infected' may include 'dis_stage_1',
-'dis_stage_2' and 'dis_advanced', where 'dis_advanced' is another
-previously-defined characteristic including 'dis_stage_3' and
-'dis_stage_4'.
-In an example model, 'infected' would track population size summed
-across the four 'dis_stage' states.
-Note: If two or more components are listed in the same column, they
-must be separated by a comma.
-Whitespace is allowable and will be deleted during processing.
-[attribute_charac_includes]</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000006000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>This column defines a 'denominator' attribute for a 'charac' item.</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000007000000}">
       <text>
         <r>
@@ -556,7 +556,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="78">
   <si>
     <t>Name</t>
   </si>
@@ -1405,7 +1405,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
@@ -1513,10 +1513,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1524,9 +1524,10 @@
     <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.7109375" customWidth="1"/>
-    <col min="4" max="5" width="20.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
     <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1544,13 +1545,13 @@
         <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>34</v>
@@ -1567,10 +1568,10 @@
         <v>6</v>
       </c>
       <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>37</v>
       </c>
+      <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="2"/>
     </row>
@@ -1585,14 +1586,16 @@
         <v>6</v>
       </c>
       <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="E3" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="F3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H3" s="2"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="2">
+        <v>10</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -1603,10 +1606,10 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>42</v>
       </c>
+      <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="2"/>
     </row>
@@ -1619,10 +1622,10 @@
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>45</v>
       </c>
+      <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="2"/>
     </row>
@@ -1635,10 +1638,10 @@
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>48</v>
       </c>
+      <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="2"/>
     </row>
@@ -1651,13 +1654,13 @@
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="E7" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="F7" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G7" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="G7" s="3"/>
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1669,13 +1672,13 @@
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="E8" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="F8" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G8" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="G8" s="3"/>
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1687,14 +1690,21 @@
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="E9" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="F9" s="3" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H9" s="2"/>
+        <v>74</v>
+      </c>
+      <c r="H9" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1707,7 +1717,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>